<commit_message>
Added check stock, write to file, some error handling for invalid orders
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyra\Documents\Term3\COMP_3522_OOP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cyra\PycharmProjects\Assignment2_A01080450_A01170735\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0417D105-D250-4F92-8142-58B494C4E488}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F5DE10-702B-4561-AB0D-67C06F22B856}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41775" yWindow="2190" windowWidth="13230" windowHeight="12720" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
+    <workbookView xWindow="34935" yWindow="2970" windowWidth="15960" windowHeight="11055" xr2:uid="{B319D853-5A99-4F7A-80BD-54EAB27A7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -663,9 +663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC969572-FB28-418E-B89D-F0DD002AE5AA}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1242,7 +1242,7 @@
         <v>69</v>
       </c>
       <c r="E15">
-        <v>13</v>
+        <v>101</v>
       </c>
       <c r="F15" t="s">
         <v>56</v>

</xml_diff>